<commit_message>
enhanced styling and search
</commit_message>
<xml_diff>
--- a/src/main/resources/registration_details.xlsx
+++ b/src/main/resources/registration_details.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27210"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7855580F-0460-4128-82EF-28BEFB264B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{95A8B5CA-46AE-4E07-9FE7-AE424F221578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>first_name</t>
   </si>
@@ -45,10 +45,37 @@
     <t>address</t>
   </si>
   <si>
-    <t>designation</t>
-  </si>
-  <si>
-    <t>Ramesh</t>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>care_of</t>
+  </si>
+  <si>
+    <t>relation</t>
+  </si>
+  <si>
+    <t>dob</t>
+  </si>
+  <si>
+    <t>registration_date</t>
+  </si>
+  <si>
+    <t>gothram</t>
+  </si>
+  <si>
+    <t>native_place</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>sub_set</t>
+  </si>
+  <si>
+    <t>married</t>
+  </si>
+  <si>
+    <t>Ramesh kumar</t>
   </si>
   <si>
     <t>Ippagunta</t>
@@ -60,13 +87,79 @@
     <t>HLC</t>
   </si>
   <si>
-    <t>Arun</t>
-  </si>
-  <si>
-    <t>Bachupally</t>
-  </si>
-  <si>
-    <t>IT</t>
+    <t>Ramesh kumar, Ippagunta</t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>kasyapasa</t>
+  </si>
+  <si>
+    <t>kandukur</t>
+  </si>
+  <si>
+    <t>niyogi</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Arun kumar</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>son</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Raghuveer</t>
+  </si>
+  <si>
+    <t>Varalakshmi</t>
+  </si>
+  <si>
+    <t>Home Maker</t>
+  </si>
+  <si>
+    <t>wife</t>
+  </si>
+  <si>
+    <t>Umamaheswara sarma</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Serilingampally</t>
+  </si>
+  <si>
+    <t>Retired in Granules India Ltd.</t>
+  </si>
+  <si>
+    <t>Umamaheswara sarma, B</t>
+  </si>
+  <si>
+    <t>koundinyasa</t>
+  </si>
+  <si>
+    <t>guntur</t>
+  </si>
+  <si>
+    <t>V. Annapurna</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>Radhakrishna</t>
   </si>
 </sst>
 </file>
@@ -102,8 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,15 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,39 +536,340 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>961079714</v>
+        <v>9618079714</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1">
+        <v>24395</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45276</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2">
+        <v>6000</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>9014038608</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36253</v>
+      </c>
+      <c r="I3" s="1">
+        <v>45277</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3">
+        <v>6000</v>
+      </c>
+      <c r="N3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>9493131211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="1">
+        <v>34575</v>
+      </c>
+      <c r="I4" s="1">
+        <v>45278</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4">
+        <v>6000</v>
+      </c>
+      <c r="N4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>9618056830</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="1">
+        <v>24513</v>
+      </c>
+      <c r="I5" s="1">
+        <v>45279</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5">
+        <v>6000</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>9949088070</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1">
+        <v>24624</v>
+      </c>
+      <c r="I6" s="1">
+        <v>45247</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6">
+        <v>6000</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>9849345243</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1">
+        <v>25729</v>
+      </c>
+      <c r="I7" s="1">
+        <v>45248</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7">
+        <v>6000</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>9963884514</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1">
+        <v>35102</v>
+      </c>
+      <c r="I8" s="1">
+        <v>45249</v>
+      </c>
+      <c r="J8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>6000</v>
+      </c>
+      <c r="N8" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>